<commit_message>
Added a "Dictionary Key" column
</commit_message>
<xml_diff>
--- a/Templete.xlsx
+++ b/Templete.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1"/>
@@ -130,6 +130,34 @@
   </si>
   <si>
     <t>1.234f</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dictionary Key</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>hoge_int</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>hoge_short</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>hoge_long</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>hoge_string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>empty_string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>if colmn "Dictionary Key" is empty, ignore convert ToDictionary()</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -168,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -191,11 +219,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -211,6 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -488,7 +528,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
@@ -499,285 +539,331 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" customWidth="1"/>
+    <col min="1" max="2" width="30.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="45.1640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="45.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F7" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="5">
+      <c r="D8" s="5">
         <v>1.234</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C10" s="2"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="2"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C12" s="2"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C13" s="2"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C14" s="2"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C15" s="2"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C16" s="2"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="2"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="2"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="2"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="2"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C21" s="2"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C22" s="2"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C23" s="2"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C24" s="2"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C25" s="2"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C26" s="2"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C27" s="2"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C28" s="2"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C29" s="2"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C30" s="2"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C31" s="2"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C32" s="2"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B33">
-      <formula1>"byte,short,int,long,float,double,string"</formula1>
-    </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C9:C33"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="C2:C4" numberStoredAsText="1"/>
+    <ignoredError sqref="D2:D4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Multi sheets convert supported Classname generate from sheet’s name
</commit_message>
<xml_diff>
--- a/Templete.xlsx
+++ b/Templete.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SampleClassA" sheetId="1" r:id="rId1"/>
+    <sheet name="SampleClassB" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1"/>
@@ -41,10 +42,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -157,7 +154,15 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>if colmn "Dictionary Key" is empty, ignore convert ToDictionary()</t>
+    <t>Default Value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>if colmn "Dictionary Key" is empty,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Not generate code on ToDictionary() and CreateFromDictionary()</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -165,7 +170,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -176,6 +181,15 @@
     </font>
     <font>
       <sz val="6"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
       <charset val="128"/>
@@ -234,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -250,7 +264,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -528,7 +543,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
@@ -539,11 +554,303 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="45.1640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="45.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="33.5" customWidth="1"/>
+    <col min="1" max="2" width="30.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="45.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <dataValidations count="1">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C6:C30"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D2:D4" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="45.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -551,13 +858,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -565,121 +872,84 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>23</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1.234</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>7</v>
+        <v>24</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1.234</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
@@ -828,42 +1098,11 @@
       <c r="D29" s="5"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="2"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="1">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C9:C33"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C5:C29"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="D2:D4" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>